<commit_message>
Dados 23/24 - falta níveis de proficiência
</commit_message>
<xml_diff>
--- a/data/2223.xlsx
+++ b/data/2223.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novasbe365-my.sharepoint.com/personal/joao_correia_novasbe_pt/Documents/Documentos/AoL2324/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="126" documentId="8_{3FE0FD0C-8F14-4414-B34C-E567F4A11488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C519EF86-134E-4035-A9A4-AEBBB8199D73}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{3FE0FD0C-8F14-4414-B34C-E567F4A11488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95AFAB1A-70BD-4E4D-A00B-948D9686E44A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{20674098-312E-49A1-8D81-C0338F29F4BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$42</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="12">
   <si>
     <t>Program</t>
   </si>
@@ -69,6 +72,9 @@
   </si>
   <si>
     <t>VI</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BBE84B6-830C-4E4E-B99C-BCCB0BEC31F1}">
-  <dimension ref="A1:C41"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -470,7 +477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -481,7 +488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -492,7 +499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -503,7 +510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -514,7 +521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -525,7 +532,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -536,7 +543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -547,7 +554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -558,7 +565,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>14</v>
       </c>
@@ -569,7 +576,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>14</v>
       </c>
@@ -580,7 +587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>14</v>
       </c>
@@ -591,7 +598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>14</v>
       </c>
@@ -602,7 +609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>15</v>
       </c>
@@ -613,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -624,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -635,7 +642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -646,7 +653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -657,7 +664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -668,7 +675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -679,7 +686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>16</v>
       </c>
@@ -734,7 +741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>38</v>
       </c>
@@ -745,7 +752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>38</v>
       </c>
@@ -756,7 +763,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>38</v>
       </c>
@@ -767,7 +774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>38</v>
       </c>
@@ -778,7 +785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>39</v>
       </c>
@@ -789,7 +796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>39</v>
       </c>
@@ -800,7 +807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>39</v>
       </c>
@@ -811,7 +818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>39</v>
       </c>
@@ -822,7 +829,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>27</v>
       </c>
@@ -833,7 +840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>27</v>
       </c>
@@ -844,7 +851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>27</v>
       </c>
@@ -855,7 +862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>27</v>
       </c>
@@ -866,7 +873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>33</v>
       </c>
@@ -877,7 +884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>33</v>
       </c>
@@ -888,7 +895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>33</v>
       </c>
@@ -899,7 +906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>33</v>
       </c>
@@ -910,7 +917,36 @@
         <v>7</v>
       </c>
     </row>
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>39</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>37</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:C42" xr:uid="{1BBE84B6-830C-4E4E-B99C-BCCB0BEC31F1}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="37"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
small correction in the 2223 data
</commit_message>
<xml_diff>
--- a/data/2223.xlsx
+++ b/data/2223.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novasbe365-my.sharepoint.com/personal/joao_correia_novasbe_pt/Documents/Documentos/AoL2324/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{3FE0FD0C-8F14-4414-B34C-E567F4A11488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95AFAB1A-70BD-4E4D-A00B-948D9686E44A}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{3FE0FD0C-8F14-4414-B34C-E567F4A11488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0A5127D-5805-4F60-8F42-E5B66BABFB93}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{20674098-312E-49A1-8D81-C0338F29F4BF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20674098-312E-49A1-8D81-C0338F29F4BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -458,7 +458,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -477,7 +477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -485,10 +485,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -499,7 +499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -510,7 +510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -521,7 +521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -529,10 +529,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -543,7 +543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -554,7 +554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -697,7 +697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>37</v>
       </c>
@@ -708,7 +708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>37</v>
       </c>
@@ -719,7 +719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>37</v>
       </c>
@@ -730,7 +730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>37</v>
       </c>
@@ -928,7 +928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>37</v>
       </c>
@@ -940,10 +940,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C42" xr:uid="{1BBE84B6-830C-4E4E-B99C-BCCB0BEC31F1}">
+  <autoFilter ref="A1:C43" xr:uid="{1BBE84B6-830C-4E4E-B99C-BCCB0BEC31F1}">
     <filterColumn colId="0">
       <filters>
-        <filter val="37"/>
+        <filter val="1"/>
+        <filter val="2"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
versão final do relatório AoL2023/2024
</commit_message>
<xml_diff>
--- a/data/2223.xlsx
+++ b/data/2223.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novasbe365-my.sharepoint.com/personal/joao_correia_novasbe_pt/Documents/Documentos/AoL2324/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Correia\OneDrive - Nova SBE\Documentos\AoL2324\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{3FE0FD0C-8F14-4414-B34C-E567F4A11488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0A5127D-5805-4F60-8F42-E5B66BABFB93}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D3C5DF-E9A4-4C0A-9C99-7661C2A2381F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20674098-312E-49A1-8D81-C0338F29F4BF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{20674098-312E-49A1-8D81-C0338F29F4BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -485,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -529,7 +529,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>